<commit_message>
Atualizado Lista Componentes.xlsx. Atualizado cálculos conversor BOOST. Adicionado arquivos.
</commit_message>
<xml_diff>
--- a/documentos/Lista Componentes.xlsx
+++ b/documentos/Lista Componentes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>Data</t>
   </si>
@@ -67,6 +67,30 @@
   </si>
   <si>
     <t>Mundial Componentes</t>
+  </si>
+  <si>
+    <t>16/112012</t>
+  </si>
+  <si>
+    <t>CONECTOR modu 2542</t>
+  </si>
+  <si>
+    <t>TERMINAL para conector modu 22/26AWG</t>
+  </si>
+  <si>
+    <t>CABO FLAT de fio 10 vias</t>
+  </si>
+  <si>
+    <t>IMPRESSÃO</t>
+  </si>
+  <si>
+    <t>PAPEL GLOSSY</t>
+  </si>
+  <si>
+    <t>Papelaria</t>
+  </si>
+  <si>
+    <t>Copia IFSC</t>
   </si>
 </sst>
 </file>
@@ -153,9 +177,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -171,6 +192,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -467,10 +491,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -484,230 +509,456 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>41187</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0.3</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>5</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="4">
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3">
         <f>PRODUCT(C2:D2)</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>41187</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>1.6</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>2</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="5">
-        <f t="shared" ref="F3:F10" si="0">PRODUCT(C3:D3)</f>
+      <c r="E3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F9" si="0">PRODUCT(C3:D3)</f>
         <v>3.2</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>41187</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>1.65</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>1</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3">
         <f t="shared" si="0"/>
         <v>1.65</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>41187</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>2.5</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="5">
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>41187</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>2.25</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>6</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="4">
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3">
         <f t="shared" si="0"/>
         <v>13.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>41187</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>0.5</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>3</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="5">
+      <c r="E7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="4">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>41187</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>0.5</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>3</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="4">
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>41187</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>0.5</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>3</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="5">
+      <c r="E9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="4">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>41187</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>0.5</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>3</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="4">
-        <f t="shared" si="0"/>
+      <c r="E10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" ref="F10:F26" si="1">PRODUCT(C10:D10)</f>
         <v>1.5</v>
       </c>
     </row>
+    <row r="11" spans="1:6" ht="15.75">
+      <c r="A11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D11" s="4">
+        <v>4</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="1"/>
+        <v>2.4</v>
+      </c>
+    </row>
     <row r="12" spans="1:6" ht="15.75">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>16</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="1"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75">
+      <c r="A13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75">
+      <c r="A14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="D14" s="3">
+        <v>37</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="1"/>
+        <v>5.55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75">
+      <c r="A15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75">
+      <c r="A16" s="5"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75">
+      <c r="A17" s="6"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75">
+      <c r="A18" s="5"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75">
+      <c r="A19" s="6"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75">
+      <c r="A20" s="5"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75">
+      <c r="A21" s="6"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75">
+      <c r="A22" s="5"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75">
+      <c r="A23" s="6"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75">
+      <c r="A24" s="5"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75">
+      <c r="A25" s="6"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75">
+      <c r="A26" s="5"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75">
+      <c r="A28" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="1">
-        <f>SUM(F2:F10)</f>
-        <v>28.35</v>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="1">
+        <f>SUM(F2:F26)</f>
+        <v>41.9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A28:E28"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização da lista de componentes. Adicionado datasheet do regulador 78RM33 adquirido.
</commit_message>
<xml_diff>
--- a/documentos/Lista Componentes.xlsx
+++ b/documentos/Lista Componentes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>Data</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>Copia IFSC</t>
+  </si>
+  <si>
+    <t>Regulador 74RM33</t>
+  </si>
+  <si>
+    <t>SOQUETE torneado 28 pinos</t>
+  </si>
+  <si>
+    <t>74HC125 BUS Line Driver</t>
   </si>
 </sst>
 </file>
@@ -491,11 +500,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -713,7 +722,7 @@
         <v>16</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" ref="F10:F26" si="1">PRODUCT(C10:D10)</f>
+        <f t="shared" ref="F10:F27" si="1">PRODUCT(C10:D10)</f>
         <v>1.5</v>
       </c>
     </row>
@@ -823,142 +832,203 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75">
-      <c r="A16" s="5"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3">
+      <c r="A16" s="6">
+        <v>41239</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" ref="F16:F20" si="2">PRODUCT(C16:D16)</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75">
+      <c r="A17" s="5">
+        <v>41243</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D17" s="3">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75">
+      <c r="A18" s="6">
+        <v>41243</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="4">
+        <v>3</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75">
+      <c r="A19" s="5">
+        <v>41243</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75">
+      <c r="A20" s="6">
+        <v>41243</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D20" s="4">
+        <v>16</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="4">
+        <f t="shared" si="2"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75">
+      <c r="A21" s="5"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75">
-      <c r="A17" s="6"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4">
+    <row r="22" spans="1:6" ht="15.75">
+      <c r="A22" s="6"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75">
-      <c r="A18" s="5"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3">
+    <row r="23" spans="1:6" ht="15.75">
+      <c r="A23" s="5"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75">
-      <c r="A19" s="6"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4">
+    <row r="24" spans="1:6" ht="15.75">
+      <c r="A24" s="6"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75">
-      <c r="A20" s="5"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3">
+    <row r="25" spans="1:6" ht="15.75">
+      <c r="A25" s="5"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75">
-      <c r="A21" s="6"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4">
+    <row r="26" spans="1:6" ht="15.75">
+      <c r="A26" s="6"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75">
-      <c r="A22" s="5"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3">
+    <row r="27" spans="1:6" ht="15.75">
+      <c r="A27" s="5"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75">
-      <c r="A23" s="6"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75">
-      <c r="A24" s="5"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75">
-      <c r="A25" s="6"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75">
-      <c r="A26" s="5"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75">
-      <c r="A28" s="8" t="s">
+    <row r="29" spans="1:6" ht="15.75">
+      <c r="A29" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="1">
-        <f>SUM(F2:F26)</f>
-        <v>41.9</v>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="1">
+        <f>SUM(F2:F27)</f>
+        <v>57.2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A29:E29"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>